<commit_message>
Se elimina el access_token
</commit_message>
<xml_diff>
--- a/IA-Luján/data/papers/20230919-174050-Ambiente/indicadores.xlsx
+++ b/IA-Luján/data/papers/20230919-174050-Ambiente/indicadores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>3er Término Más Utilizado</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Resumen</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -493,6 +498,11 @@
           <t>naciones</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>['Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -522,6 +532,11 @@
           <t>medio</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -551,6 +566,11 @@
           <t>medio</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>['Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -580,6 +600,11 @@
           <t>01</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>['Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -609,6 +634,11 @@
           <t>paises</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -638,6 +668,11 @@
           <t>territorio</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>['Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -665,6 +700,11 @@
       <c r="G8" t="inlineStr">
         <is>
           <t>ambiente</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>['Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio', 'Medio Ambiente, Medio Ambiente Ambiente Medio Medio Medio Ambiente Medio Ambiente ambiente Medio Medio ambiente Medio Ambiente Natural Medio Medio Natural Medio Ambiente medio Ambiente Medio ambiente ambiente Medio ambiente Ambiente Medio espacio Medio Ambiente. Medio Ambiente Eco Medio Ambiente espacio Medio Medio medio Medio Ambiente que Medio Ambiente Marina Medio Medio Eco Medio Medio espacio Ambiente Medio medio ambiente Medio']</t>
         </is>
       </c>
     </row>

</xml_diff>